<commit_message>
Subida de Backlog completo - fabiola Benitez
</commit_message>
<xml_diff>
--- a/Documentacion/ProductBacklog.xlsx
+++ b/Documentacion/ProductBacklog.xlsx
@@ -1,20 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FABIOLA\Desktop\Proyecto Final ISPC 2023\Documentacion\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9660"/>
-  </bookViews>
   <sheets>
-    <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Product Backlog" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjVXku3GB2bzcm3AbpixQxNV+JdAA=="/>
@@ -24,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="131">
   <si>
     <t>Plantilla de historias de usuario Proyecto 2022</t>
   </si>
@@ -37,19 +29,19 @@
   <si>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <b/>
-        <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <sz val="14.0"/>
       </rPr>
       <t xml:space="preserve">Quiero </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <i/>
-        <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <sz val="14.0"/>
       </rPr>
       <t>&lt;realizar alguna tarea&gt;</t>
     </r>
@@ -57,20 +49,21 @@
   <si>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <b/>
         <i/>
-        <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <sz val="14.0"/>
       </rPr>
       <t>para que pueda</t>
     </r>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
+        <b val="0"/>
         <i/>
-        <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <sz val="14.0"/>
       </rPr>
       <t xml:space="preserve"> &lt;lograr algún objetivo&gt;</t>
     </r>
@@ -258,19 +251,19 @@
   <si>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <b/>
-        <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <sz val="14.0"/>
       </rPr>
       <t xml:space="preserve">Quiero </t>
     </r>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <i/>
-        <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <sz val="14.0"/>
       </rPr>
       <t>&lt;realizar alguna tarea&gt;</t>
     </r>
@@ -278,20 +271,21 @@
   <si>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
         <b/>
         <i/>
-        <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <sz val="14.0"/>
       </rPr>
       <t>para que pueda</t>
     </r>
     <r>
       <rPr>
+        <rFont val="Calibri"/>
+        <b val="0"/>
         <i/>
-        <sz val="14"/>
         <color theme="1"/>
-        <rFont val="Calibri"/>
+        <sz val="14.0"/>
       </rPr>
       <t xml:space="preserve"> &lt;lograr algún objetivo&gt;</t>
     </r>
@@ -465,79 +459,99 @@
     <t>US0023</t>
   </si>
   <si>
+    <t>Administrador</t>
+  </si>
+  <si>
+    <t xml:space="preserve">quiero saber que productos fueron los que mas llamaron la atención del usuario </t>
+  </si>
+  <si>
+    <t xml:space="preserve">para poder tener mayores ventas </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jesica Amaya </t>
+  </si>
+  <si>
     <t>US0024</t>
+  </si>
+  <si>
+    <t>necesito q en cada producto me informe cuantas unidades en stock quedan disponibles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">para poder hacer control y reposición de cada producto </t>
+  </si>
+  <si>
+    <t>Jesica Amaya</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <fonts count="12">
     <font>
-      <sz val="12"/>
+      <sz val="12.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="12.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="18"/>
+      <sz val="18.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="14.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <i/>
-      <sz val="14"/>
+      <sz val="14.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="14.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
       <i/>
-      <sz val="14"/>
+      <sz val="14.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="12"/>
+      <sz val="12.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF222222"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="12"/>
+      <sz val="12.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
+      <sz val="12.0"/>
       <color rgb="FF000000"/>
       <name val="Docs-Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
@@ -548,7 +562,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -570,19 +584,12 @@
     </fill>
   </fills>
   <borders count="6">
+    <border/>
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -597,7 +604,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -609,11 +615,8 @@
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
-      <bottom/>
-      <diagonal/>
     </border>
     <border>
-      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -623,7 +626,6 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -632,100 +634,117 @@
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
-      <top/>
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
   <cellXfs count="32">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="2" fillId="3" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="2" fillId="3" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="2" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="2" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="9" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf borderId="2" fillId="3" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf borderId="0" fillId="4" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf borderId="2" fillId="0" fontId="11" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -915,27 +934,27 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K1000"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="11.22" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="20" customWidth="1"/>
-    <col min="2" max="2" width="37.125" customWidth="1"/>
-    <col min="3" max="3" width="93.5" customWidth="1"/>
-    <col min="4" max="4" width="69.875" customWidth="1"/>
-    <col min="5" max="6" width="11.25" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="20.0"/>
+    <col customWidth="1" min="2" max="2" width="37.11"/>
+    <col customWidth="1" min="3" max="3" width="93.44"/>
+    <col customWidth="1" min="4" max="4" width="69.89"/>
+    <col customWidth="1" min="5" max="6" width="11.22"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" customHeight="1">
+    <row r="1" ht="15.75" customHeight="1">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -948,7 +967,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" customHeight="1">
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -963,7 +982,7 @@
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
     </row>
-    <row r="3" spans="1:11" ht="15.75" customHeight="1">
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -976,7 +995,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="15.75" customHeight="1">
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -989,7 +1008,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" ht="15.75" customHeight="1">
+    <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>1</v>
       </c>
@@ -1010,7 +1029,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" ht="21.75" customHeight="1">
+    <row r="6" ht="21.75" customHeight="1">
       <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
@@ -1031,7 +1050,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" ht="21.75" customHeight="1">
+    <row r="7" ht="21.75" customHeight="1">
       <c r="A7" s="7" t="s">
         <v>9</v>
       </c>
@@ -1052,7 +1071,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" ht="21.75" customHeight="1">
+    <row r="8" ht="21.75" customHeight="1">
       <c r="A8" s="7" t="s">
         <v>12</v>
       </c>
@@ -1073,7 +1092,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" ht="21.75" customHeight="1">
+    <row r="9" ht="21.75" customHeight="1">
       <c r="A9" s="7" t="s">
         <v>14</v>
       </c>
@@ -1094,7 +1113,7 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="1:11" ht="21.75" customHeight="1">
+    <row r="10" ht="21.75" customHeight="1">
       <c r="A10" s="7" t="s">
         <v>17</v>
       </c>
@@ -1115,7 +1134,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" ht="21.75" customHeight="1">
+    <row r="11" ht="21.75" customHeight="1">
       <c r="A11" s="7" t="s">
         <v>20</v>
       </c>
@@ -1136,7 +1155,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" ht="21.75" customHeight="1">
+    <row r="12" ht="21.75" customHeight="1">
       <c r="A12" s="7" t="s">
         <v>23</v>
       </c>
@@ -1157,7 +1176,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" ht="21.75" customHeight="1">
+    <row r="13" ht="21.75" customHeight="1">
       <c r="A13" s="7" t="s">
         <v>26</v>
       </c>
@@ -1178,7 +1197,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
     </row>
-    <row r="14" spans="1:11" ht="21.75" customHeight="1">
+    <row r="14" ht="21.75" customHeight="1">
       <c r="A14" s="7" t="s">
         <v>28</v>
       </c>
@@ -1199,7 +1218,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
     </row>
-    <row r="15" spans="1:11" ht="21.75" customHeight="1">
+    <row r="15" ht="21.75" customHeight="1">
       <c r="A15" s="7" t="s">
         <v>31</v>
       </c>
@@ -1220,7 +1239,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:11" ht="21.75" customHeight="1">
+    <row r="16" ht="21.75" customHeight="1">
       <c r="A16" s="7" t="s">
         <v>34</v>
       </c>
@@ -1241,7 +1260,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" ht="21.75" customHeight="1">
+    <row r="17" ht="21.75" customHeight="1">
       <c r="A17" s="7" t="s">
         <v>37</v>
       </c>
@@ -1262,7 +1281,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" ht="21.75" customHeight="1">
+    <row r="18" ht="21.75" customHeight="1">
       <c r="A18" s="7" t="s">
         <v>40</v>
       </c>
@@ -1283,7 +1302,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="1:11" ht="21.75" customHeight="1">
+    <row r="19" ht="21.75" customHeight="1">
       <c r="A19" s="7" t="s">
         <v>43</v>
       </c>
@@ -1304,7 +1323,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="1:11" ht="21.75" customHeight="1">
+    <row r="20" ht="21.75" customHeight="1">
       <c r="A20" s="7" t="s">
         <v>46</v>
       </c>
@@ -1325,7 +1344,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" customHeight="1">
+    <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="7" t="s">
         <v>49</v>
       </c>
@@ -1346,7 +1365,7 @@
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" customHeight="1">
+    <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="7" t="s">
         <v>52</v>
       </c>
@@ -1367,7 +1386,7 @@
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" customHeight="1">
+    <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="7" t="s">
         <v>54</v>
       </c>
@@ -1388,7 +1407,7 @@
       <c r="J23" s="1"/>
       <c r="K23" s="1"/>
     </row>
-    <row r="24" spans="1:11" ht="15.75" customHeight="1">
+    <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="7" t="s">
         <v>58</v>
       </c>
@@ -1409,7 +1428,7 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
     </row>
-    <row r="25" spans="1:11" ht="15.75" customHeight="1">
+    <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="7" t="s">
         <v>61</v>
       </c>
@@ -1430,7 +1449,7 @@
       <c r="J25" s="1"/>
       <c r="K25" s="1"/>
     </row>
-    <row r="26" spans="1:11" ht="15.75" customHeight="1">
+    <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -1443,7 +1462,7 @@
       <c r="J26" s="1"/>
       <c r="K26" s="1"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" customHeight="1">
+    <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="1"/>
       <c r="B27" s="13"/>
       <c r="C27" s="1"/>
@@ -1456,7 +1475,7 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
     </row>
-    <row r="28" spans="1:11" ht="15.75" customHeight="1">
+    <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -1469,7 +1488,7 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
     </row>
-    <row r="29" spans="1:11" ht="15.75" customHeight="1">
+    <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="14" t="s">
         <v>64</v>
       </c>
@@ -1484,7 +1503,7 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
     </row>
-    <row r="30" spans="1:11" ht="15.75" customHeight="1">
+    <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -1497,7 +1516,7 @@
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
     </row>
-    <row r="31" spans="1:11" ht="15.75" customHeight="1">
+    <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="3" t="s">
         <v>1</v>
       </c>
@@ -1520,7 +1539,7 @@
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
     </row>
-    <row r="32" spans="1:11" ht="15.75" customHeight="1">
+    <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="7" t="s">
         <v>5</v>
       </c>
@@ -1543,7 +1562,7 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
     </row>
-    <row r="33" spans="1:11" ht="15.75" customHeight="1">
+    <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="7" t="s">
         <v>9</v>
       </c>
@@ -1566,7 +1585,7 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
     </row>
-    <row r="34" spans="1:11" ht="15.75" customHeight="1">
+    <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="7" t="s">
         <v>12</v>
       </c>
@@ -1589,7 +1608,7 @@
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
     </row>
-    <row r="35" spans="1:11" ht="15.75" customHeight="1">
+    <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="7" t="s">
         <v>14</v>
       </c>
@@ -1612,7 +1631,7 @@
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
     </row>
-    <row r="36" spans="1:11" ht="15.75" customHeight="1">
+    <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="7" t="s">
         <v>17</v>
       </c>
@@ -1635,7 +1654,7 @@
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
-    <row r="37" spans="1:11" ht="15.75" customHeight="1">
+    <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="7" t="s">
         <v>20</v>
       </c>
@@ -1658,7 +1677,7 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
     </row>
-    <row r="38" spans="1:11" ht="15.75" customHeight="1">
+    <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="7" t="s">
         <v>23</v>
       </c>
@@ -1681,7 +1700,7 @@
       <c r="J38" s="1"/>
       <c r="K38" s="1"/>
     </row>
-    <row r="39" spans="1:11" ht="15.75" customHeight="1">
+    <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="7" t="s">
         <v>26</v>
       </c>
@@ -1704,7 +1723,7 @@
       <c r="J39" s="1"/>
       <c r="K39" s="1"/>
     </row>
-    <row r="40" spans="1:11" ht="15.75" customHeight="1">
+    <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="7" t="s">
         <v>28</v>
       </c>
@@ -1727,7 +1746,7 @@
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
     </row>
-    <row r="41" spans="1:11" ht="15.75" customHeight="1">
+    <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="7" t="s">
         <v>31</v>
       </c>
@@ -1750,7 +1769,7 @@
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
     </row>
-    <row r="42" spans="1:11" ht="15.75" customHeight="1">
+    <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="7" t="s">
         <v>34</v>
       </c>
@@ -1773,7 +1792,7 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
     </row>
-    <row r="43" spans="1:11" ht="15.75" customHeight="1">
+    <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="7" t="s">
         <v>37</v>
       </c>
@@ -1796,7 +1815,7 @@
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
     </row>
-    <row r="44" spans="1:11" ht="15.75" customHeight="1">
+    <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="7" t="s">
         <v>40</v>
       </c>
@@ -1819,7 +1838,7 @@
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
     </row>
-    <row r="45" spans="1:11" ht="15.75" customHeight="1">
+    <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="7" t="s">
         <v>43</v>
       </c>
@@ -1842,7 +1861,7 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
     </row>
-    <row r="46" spans="1:11" ht="15.75" customHeight="1">
+    <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="7" t="s">
         <v>46</v>
       </c>
@@ -1865,7 +1884,7 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
     </row>
-    <row r="47" spans="1:11" ht="15.75" customHeight="1">
+    <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="7" t="s">
         <v>49</v>
       </c>
@@ -1888,7 +1907,7 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
     </row>
-    <row r="48" spans="1:11" ht="15.75" customHeight="1">
+    <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="7" t="s">
         <v>52</v>
       </c>
@@ -1911,7 +1930,7 @@
       <c r="J48" s="1"/>
       <c r="K48" s="1"/>
     </row>
-    <row r="49" spans="1:11" ht="15.75" customHeight="1">
+    <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="7" t="s">
         <v>54</v>
       </c>
@@ -1934,7 +1953,7 @@
       <c r="J49" s="1"/>
       <c r="K49" s="1"/>
     </row>
-    <row r="50" spans="1:11" ht="15.75" customHeight="1">
+    <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="7" t="s">
         <v>58</v>
       </c>
@@ -1957,7 +1976,7 @@
       <c r="J50" s="1"/>
       <c r="K50" s="1"/>
     </row>
-    <row r="51" spans="1:11" ht="15.75" customHeight="1">
+    <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="7" t="s">
         <v>61</v>
       </c>
@@ -1980,7 +1999,7 @@
       <c r="J51" s="1"/>
       <c r="K51" s="1"/>
     </row>
-    <row r="52" spans="1:11" ht="15.75" customHeight="1">
+    <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="16" t="s">
         <v>116</v>
       </c>
@@ -2003,7 +2022,7 @@
       <c r="J52" s="1"/>
       <c r="K52" s="1"/>
     </row>
-    <row r="53" spans="1:11" ht="15.75" customHeight="1">
+    <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="27" t="s">
         <v>119</v>
       </c>
@@ -2026,14 +2045,22 @@
       <c r="J53" s="1"/>
       <c r="K53" s="1"/>
     </row>
-    <row r="54" spans="1:11" ht="15.75" customHeight="1">
+    <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="27" t="s">
         <v>122</v>
       </c>
-      <c r="B54" s="7"/>
-      <c r="C54" s="11"/>
-      <c r="D54" s="11"/>
-      <c r="E54" s="18"/>
+      <c r="B54" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C54" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="D54" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="E54" s="18" t="s">
+        <v>126</v>
+      </c>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
       <c r="H54" s="1"/>
@@ -2041,14 +2068,22 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
     </row>
-    <row r="55" spans="1:11" ht="15.75" customHeight="1">
+    <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="27" t="s">
+        <v>127</v>
+      </c>
+      <c r="B55" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="B55" s="7"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="18"/>
+      <c r="C55" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="D55" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="E55" s="18" t="s">
+        <v>130</v>
+      </c>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
       <c r="H55" s="1"/>
@@ -2056,7 +2091,7 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
     </row>
-    <row r="56" spans="1:11" ht="15.75" customHeight="1">
+    <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="31"/>
       <c r="B56" s="31"/>
       <c r="C56" s="31"/>
@@ -2069,7 +2104,7 @@
       <c r="J56" s="1"/>
       <c r="K56" s="1"/>
     </row>
-    <row r="57" spans="1:11" ht="15.75" customHeight="1">
+    <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="1"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2082,7 +2117,7 @@
       <c r="J57" s="1"/>
       <c r="K57" s="1"/>
     </row>
-    <row r="58" spans="1:11" ht="15.75" customHeight="1">
+    <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="1"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2095,7 +2130,7 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
     </row>
-    <row r="59" spans="1:11" ht="15.75" customHeight="1">
+    <row r="59" ht="15.75" customHeight="1">
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -2104,7 +2139,7 @@
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
     </row>
-    <row r="60" spans="1:11" ht="15.75" customHeight="1">
+    <row r="60" ht="15.75" customHeight="1">
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -2113,7 +2148,7 @@
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
     </row>
-    <row r="61" spans="1:11" ht="15.75" customHeight="1">
+    <row r="61" ht="15.75" customHeight="1">
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -2122,7 +2157,7 @@
       <c r="J61" s="1"/>
       <c r="K61" s="1"/>
     </row>
-    <row r="62" spans="1:11" ht="15.75" customHeight="1">
+    <row r="62" ht="15.75" customHeight="1">
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -2131,7 +2166,7 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
     </row>
-    <row r="63" spans="1:11" ht="15.75" customHeight="1">
+    <row r="63" ht="15.75" customHeight="1">
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -2140,7 +2175,7 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
     </row>
-    <row r="64" spans="1:11" ht="15.75" customHeight="1">
+    <row r="64" ht="15.75" customHeight="1">
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -2149,7 +2184,7 @@
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
     </row>
-    <row r="65" spans="5:11" ht="15.75" customHeight="1">
+    <row r="65" ht="15.75" customHeight="1">
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -2158,21 +2193,21 @@
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
     </row>
-    <row r="66" spans="5:11" ht="15.75" customHeight="1"/>
-    <row r="67" spans="5:11" ht="15.75" customHeight="1"/>
-    <row r="68" spans="5:11" ht="15.75" customHeight="1"/>
-    <row r="69" spans="5:11" ht="15.75" customHeight="1"/>
-    <row r="70" spans="5:11" ht="15.75" customHeight="1"/>
-    <row r="71" spans="5:11" ht="15.75" customHeight="1"/>
-    <row r="72" spans="5:11" ht="15.75" customHeight="1"/>
-    <row r="73" spans="5:11" ht="15.75" customHeight="1"/>
-    <row r="74" spans="5:11" ht="15.75" customHeight="1"/>
-    <row r="75" spans="5:11" ht="15.75" customHeight="1"/>
-    <row r="76" spans="5:11" ht="15.75" customHeight="1"/>
-    <row r="77" spans="5:11" ht="15.75" customHeight="1"/>
-    <row r="78" spans="5:11" ht="15.75" customHeight="1"/>
-    <row r="79" spans="5:11" ht="15.75" customHeight="1"/>
-    <row r="80" spans="5:11" ht="15.75" customHeight="1"/>
+    <row r="66" ht="15.75" customHeight="1"/>
+    <row r="67" ht="15.75" customHeight="1"/>
+    <row r="68" ht="15.75" customHeight="1"/>
+    <row r="69" ht="15.75" customHeight="1"/>
+    <row r="70" ht="15.75" customHeight="1"/>
+    <row r="71" ht="15.75" customHeight="1"/>
+    <row r="72" ht="15.75" customHeight="1"/>
+    <row r="73" ht="15.75" customHeight="1"/>
+    <row r="74" ht="15.75" customHeight="1"/>
+    <row r="75" ht="15.75" customHeight="1"/>
+    <row r="76" ht="15.75" customHeight="1"/>
+    <row r="77" ht="15.75" customHeight="1"/>
+    <row r="78" ht="15.75" customHeight="1"/>
+    <row r="79" ht="15.75" customHeight="1"/>
+    <row r="80" ht="15.75" customHeight="1"/>
     <row r="81" ht="15.75" customHeight="1"/>
     <row r="82" ht="15.75" customHeight="1"/>
     <row r="83" ht="15.75" customHeight="1"/>
@@ -3094,7 +3129,9 @@
     <row r="999" ht="15.75" customHeight="1"/>
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
+  <printOptions/>
+  <pageMargins bottom="1.0" footer="0.0" header="0.0" left="0.75" right="0.75" top="1.0"/>
   <pageSetup orientation="portrait"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>